<commit_message>
up - final pandas
</commit_message>
<xml_diff>
--- a/01_bigData_RealTime_Python_Spark/cap03_Pandas/dados/df_resumo_performance_escolar.xlsx
+++ b/01_bigData_RealTime_Python_Spark/cap03_Pandas/dados/df_resumo_performance_escolar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmpm/Dropbox/DSA/BigDataAnalytics-Python-Spark/Cap03/dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\formacao_dataScience_DSA\01_bigData_RealTime_Python_Spark\cap03_Pandas\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423FB373-9D9E-C741-AF9C-364036BCA3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081296E6-5997-4A82-8C79-DEF6DCB3447F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="3040" windowWidth="25300" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,9 +296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -336,9 +336,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,26 +371,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,26 +406,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,26 +585,26 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -711,7 +677,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -749,7 +715,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -787,7 +753,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -825,7 +791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -863,7 +829,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -901,7 +867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -939,7 +905,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -977,7 +943,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +981,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1053,7 +1019,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1057,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1129,7 +1095,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1167,7 +1133,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1205,7 +1171,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>